<commit_message>
Added condition that input amount must be >= 0 + test for this. Finally final version :).
</commit_message>
<xml_diff>
--- a/entry-task/cur_symbols/c_symbols.xlsx
+++ b/entry-task/cur_symbols/c_symbols.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="706">
   <si>
     <t>MKD</t>
   </si>
@@ -2137,6 +2137,9 @@
   </si>
   <si>
     <t>som</t>
+  </si>
+  <si>
+    <t>SFr.</t>
   </si>
 </sst>
 </file>
@@ -2969,8 +2972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C87" sqref="A1:C112"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3896,13 +3899,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>449</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>705</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>448</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="2"/>
@@ -3923,13 +3926,13 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>202</v>
+        <v>9</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>203</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>204</v>
+        <v>11</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="2"/>
@@ -3950,13 +3953,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>155</v>
+        <v>203</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="2"/>
@@ -3977,13 +3980,13 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="2"/>
@@ -4004,13 +4007,13 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>394</v>
-      </c>
-      <c r="B39" t="s">
-        <v>393</v>
+        <v>75</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>392</v>
+        <v>77</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="2"/>
@@ -4026,18 +4029,18 @@
       </c>
       <c r="K39" t="str">
         <f t="shared" si="5"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>25</v>
+        <v>394</v>
+      </c>
+      <c r="B40" t="s">
+        <v>393</v>
       </c>
       <c r="C40" t="s">
-        <v>26</v>
+        <v>392</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="2"/>
@@ -4049,19 +4052,19 @@
       </c>
       <c r="J40" t="str">
         <f t="shared" si="4"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
-      <c r="B41" t="s">
-        <v>414</v>
+      <c r="B41" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C41" t="s">
         <v>26</v>
@@ -4085,13 +4088,13 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>142</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>143</v>
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>414</v>
       </c>
       <c r="C42" t="s">
-        <v>144</v>
+        <v>26</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="2"/>
@@ -4103,7 +4106,7 @@
       </c>
       <c r="J42" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="5"/>
@@ -4112,13 +4115,13 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="2"/>
@@ -4139,13 +4142,13 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="2"/>
@@ -4166,13 +4169,13 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>172</v>
+        <v>57</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>173</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>174</v>
+        <v>59</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="2"/>
@@ -4193,13 +4196,13 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="C46" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="2"/>
@@ -4220,13 +4223,13 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="2"/>
@@ -4247,13 +4250,13 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="2"/>
@@ -4274,13 +4277,13 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>257</v>
+        <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="2"/>
@@ -4296,18 +4299,18 @@
       </c>
       <c r="K49" t="str">
         <f t="shared" si="5"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>149</v>
+        <v>257</v>
       </c>
       <c r="C50" t="s">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="2"/>
@@ -4323,18 +4326,18 @@
       </c>
       <c r="K50" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>148</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
       <c r="C51" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="2"/>
@@ -4346,7 +4349,7 @@
       </c>
       <c r="J51" t="str">
         <f t="shared" si="4"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="5"/>
@@ -4357,8 +4360,8 @@
       <c r="A52" t="s">
         <v>199</v>
       </c>
-      <c r="B52" t="s">
-        <v>438</v>
+      <c r="B52" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="C52" t="s">
         <v>201</v>
@@ -4382,13 +4385,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>598</v>
+        <v>199</v>
       </c>
       <c r="B53" t="s">
-        <v>697</v>
+        <v>438</v>
       </c>
       <c r="C53" t="s">
-        <v>596</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -4396,7 +4399,7 @@
         <v>598</v>
       </c>
       <c r="B54" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C54" t="s">
         <v>596</v>
@@ -4420,13 +4423,13 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>223</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>224</v>
+        <v>598</v>
+      </c>
+      <c r="B55" t="s">
+        <v>700</v>
       </c>
       <c r="C55" t="s">
-        <v>225</v>
+        <v>596</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="2"/>
@@ -4438,7 +4441,7 @@
       </c>
       <c r="J55" t="str">
         <f t="shared" ref="J55:J86" si="7">IF(COUNTIF(A:A,A55) &gt; 1, "X", "")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K55" t="str">
         <f t="shared" si="6"/>
@@ -4447,13 +4450,13 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>13</v>
+        <v>224</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="2"/>
@@ -4474,13 +4477,13 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="2"/>
@@ -4501,13 +4504,13 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>249</v>
+        <v>21</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>250</v>
+        <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>251</v>
+        <v>23</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="2"/>
@@ -4528,13 +4531,13 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C59" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="2"/>
@@ -4555,13 +4558,13 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>110</v>
+        <v>255</v>
       </c>
       <c r="C60" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" ref="H60:H80" si="8">IF(B60="","X","")</f>
@@ -4573,7 +4576,7 @@
       </c>
       <c r="J60" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K60" t="str">
         <f t="shared" si="6"/>
@@ -4584,8 +4587,8 @@
       <c r="A61" t="s">
         <v>109</v>
       </c>
-      <c r="B61" t="s">
-        <v>489</v>
+      <c r="B61" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C61" t="s">
         <v>111</v>
@@ -4609,13 +4612,13 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>211</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>212</v>
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
+        <v>489</v>
       </c>
       <c r="C62" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="8"/>
@@ -4627,7 +4630,7 @@
       </c>
       <c r="J62" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="6"/>
@@ -4636,13 +4639,13 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>259</v>
+        <v>211</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>87</v>
+        <v>212</v>
       </c>
       <c r="C63" t="s">
-        <v>88</v>
+        <v>213</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="8"/>
@@ -4663,13 +4666,13 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>259</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="8"/>
@@ -4690,13 +4693,13 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="C65" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="8"/>
@@ -4717,13 +4720,13 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="C66" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="8"/>
@@ -4735,7 +4738,7 @@
       </c>
       <c r="J66" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="6"/>
@@ -4746,8 +4749,8 @@
       <c r="A67" t="s">
         <v>15</v>
       </c>
-      <c r="B67" t="s">
-        <v>463</v>
+      <c r="B67" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -4771,13 +4774,13 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>118</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>119</v>
+        <v>15</v>
+      </c>
+      <c r="B68" t="s">
+        <v>463</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>17</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="8"/>
@@ -4789,7 +4792,7 @@
       </c>
       <c r="J68" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="6"/>
@@ -4798,13 +4801,13 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="8"/>
@@ -4825,13 +4828,13 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>128</v>
+        <v>49</v>
       </c>
       <c r="C70" t="s">
-        <v>129</v>
+        <v>50</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="8"/>
@@ -4852,13 +4855,13 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>196</v>
+        <v>127</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>197</v>
+        <v>128</v>
       </c>
       <c r="C71" t="s">
-        <v>198</v>
+        <v>129</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="8"/>
@@ -4879,13 +4882,13 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>508</v>
-      </c>
-      <c r="B72" t="s">
-        <v>507</v>
+        <v>196</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="C72" t="s">
-        <v>506</v>
+        <v>198</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="8"/>
@@ -4906,13 +4909,13 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>6</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>7</v>
+        <v>508</v>
+      </c>
+      <c r="B73" t="s">
+        <v>507</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>506</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="8"/>
@@ -4933,13 +4936,13 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>166</v>
+        <v>6</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>167</v>
+        <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>168</v>
+        <v>8</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="8"/>
@@ -4960,13 +4963,13 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="C75" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="8"/>
@@ -4987,13 +4990,13 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="C76" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="8"/>
@@ -5014,13 +5017,13 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>208</v>
+        <v>151</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>209</v>
+        <v>152</v>
       </c>
       <c r="C77" t="s">
-        <v>210</v>
+        <v>153</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="8"/>
@@ -5041,13 +5044,13 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>701</v>
-      </c>
-      <c r="B78" t="s">
-        <v>635</v>
+        <v>208</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="C78" t="s">
-        <v>634</v>
+        <v>210</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="8"/>
@@ -5068,13 +5071,13 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>214</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>215</v>
+        <v>701</v>
+      </c>
+      <c r="B79" t="s">
+        <v>635</v>
       </c>
       <c r="C79" t="s">
-        <v>216</v>
+        <v>634</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="8"/>
@@ -5095,13 +5098,13 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="C80" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="8"/>
@@ -5122,20 +5125,20 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>548</v>
-      </c>
-      <c r="B81" t="s">
-        <v>547</v>
+        <v>252</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="C81" t="s">
-        <v>546</v>
+        <v>254</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" ref="H81:H112" si="10">IF(B81="","X","")</f>
+        <f t="shared" ref="H81:H113" si="10">IF(B81="","X","")</f>
         <v/>
       </c>
       <c r="I81" t="str">
-        <f t="shared" ref="I81:I112" si="11">IF(LEN(A81)&lt;&gt;3,"X","")</f>
+        <f t="shared" ref="I81:I113" si="11">IF(LEN(A81)&lt;&gt;3,"X","")</f>
         <v/>
       </c>
       <c r="J81" t="str">
@@ -5149,13 +5152,13 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>229</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>230</v>
+        <v>548</v>
+      </c>
+      <c r="B82" t="s">
+        <v>547</v>
       </c>
       <c r="C82" t="s">
-        <v>231</v>
+        <v>546</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="10"/>
@@ -5176,13 +5179,13 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>268</v>
-      </c>
-      <c r="B83" t="s">
-        <v>695</v>
+        <v>229</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="C83" t="s">
-        <v>267</v>
+        <v>231</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="10"/>
@@ -5198,18 +5201,18 @@
       </c>
       <c r="K83" t="str">
         <f t="shared" si="6"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>184</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>185</v>
+        <v>268</v>
+      </c>
+      <c r="B84" t="s">
+        <v>695</v>
       </c>
       <c r="C84" t="s">
-        <v>186</v>
+        <v>267</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="10"/>
@@ -5225,18 +5228,18 @@
       </c>
       <c r="K84" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>568</v>
-      </c>
-      <c r="B85" t="s">
-        <v>567</v>
+        <v>184</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="C85" t="s">
-        <v>566</v>
+        <v>186</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="10"/>
@@ -5257,13 +5260,13 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>175</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>176</v>
+        <v>568</v>
+      </c>
+      <c r="B86" t="s">
+        <v>567</v>
       </c>
       <c r="C86" t="s">
-        <v>177</v>
+        <v>566</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="10"/>
@@ -5278,19 +5281,19 @@
         <v/>
       </c>
       <c r="K86" t="str">
-        <f t="shared" ref="K86:K112" si="12">IF(COUNTIF(B:B,B86) &gt; 1, "X", "")</f>
+        <f t="shared" ref="K86:K113" si="12">IF(COUNTIF(B:B,B86) &gt; 1, "X", "")</f>
         <v/>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>602</v>
-      </c>
-      <c r="B87" t="s">
-        <v>601</v>
+        <v>175</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="C87" t="s">
-        <v>600</v>
+        <v>177</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="10"/>
@@ -5311,13 +5314,13 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>187</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>188</v>
+        <v>602</v>
+      </c>
+      <c r="B88" t="s">
+        <v>601</v>
       </c>
       <c r="C88" t="s">
-        <v>189</v>
+        <v>600</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="10"/>
@@ -5338,13 +5341,13 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="C89" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="10"/>
@@ -5365,13 +5368,13 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>206</v>
+        <v>131</v>
       </c>
       <c r="C90" t="s">
-        <v>207</v>
+        <v>132</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="10"/>
@@ -5392,13 +5395,13 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C91" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="10"/>
@@ -5410,7 +5413,7 @@
       </c>
       <c r="J91" t="str">
         <f t="shared" si="13"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K91" t="str">
         <f t="shared" si="12"/>
@@ -5421,8 +5424,8 @@
       <c r="A92" t="s">
         <v>217</v>
       </c>
-      <c r="B92" t="s">
-        <v>696</v>
+      <c r="B92" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="C92" t="s">
         <v>219</v>
@@ -5446,13 +5449,13 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>220</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
+      </c>
+      <c r="B93" t="s">
+        <v>696</v>
       </c>
       <c r="C93" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="10"/>
@@ -5464,7 +5467,7 @@
       </c>
       <c r="J93" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K93" t="str">
         <f t="shared" si="12"/>
@@ -5473,13 +5476,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>98</v>
+        <v>221</v>
       </c>
       <c r="C94" t="s">
-        <v>99</v>
+        <v>222</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="10"/>
@@ -5500,13 +5503,13 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>620</v>
-      </c>
-      <c r="B95" t="s">
-        <v>619</v>
+        <v>97</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C95" t="s">
-        <v>618</v>
+        <v>99</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="10"/>
@@ -5527,13 +5530,13 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>51</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>52</v>
+        <v>620</v>
+      </c>
+      <c r="B96" t="s">
+        <v>619</v>
       </c>
       <c r="C96" t="s">
-        <v>53</v>
+        <v>618</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="10"/>
@@ -5554,13 +5557,13 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>631</v>
-      </c>
-      <c r="B97" t="s">
-        <v>630</v>
+        <v>51</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C97" t="s">
-        <v>629</v>
+        <v>53</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="10"/>
@@ -5581,13 +5584,13 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>517</v>
+        <v>631</v>
       </c>
       <c r="B98" t="s">
-        <v>702</v>
+        <v>630</v>
       </c>
       <c r="C98" t="s">
-        <v>515</v>
+        <v>629</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="10"/>
@@ -5608,13 +5611,13 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>657</v>
+        <v>517</v>
       </c>
       <c r="B99" t="s">
-        <v>656</v>
+        <v>702</v>
       </c>
       <c r="C99" t="s">
-        <v>655</v>
+        <v>515</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="10"/>
@@ -5635,13 +5638,13 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>27</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>28</v>
+        <v>657</v>
+      </c>
+      <c r="B100" t="s">
+        <v>656</v>
       </c>
       <c r="C100" t="s">
-        <v>29</v>
+        <v>655</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="10"/>
@@ -5662,13 +5665,13 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>264</v>
+        <v>27</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C101" t="s">
-        <v>265</v>
+        <v>29</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="10"/>
@@ -5689,13 +5692,13 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>669</v>
-      </c>
-      <c r="B102" t="s">
-        <v>704</v>
+        <v>264</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C102" t="s">
-        <v>667</v>
+        <v>265</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="10"/>
@@ -5716,13 +5719,13 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>18</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>19</v>
+        <v>669</v>
+      </c>
+      <c r="B103" t="s">
+        <v>704</v>
       </c>
       <c r="C103" t="s">
-        <v>20</v>
+        <v>667</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="10"/>
@@ -5743,13 +5746,13 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C104" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="10"/>
@@ -5770,13 +5773,13 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>232</v>
+        <v>40</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>233</v>
+        <v>41</v>
       </c>
       <c r="C105" t="s">
-        <v>234</v>
+        <v>42</v>
       </c>
       <c r="H105" t="str">
         <f t="shared" si="10"/>
@@ -5797,13 +5800,13 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C106" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="10"/>
@@ -5815,7 +5818,7 @@
       </c>
       <c r="J106" t="str">
         <f t="shared" si="13"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K106" t="str">
         <f t="shared" si="12"/>
@@ -5826,8 +5829,8 @@
       <c r="A107" t="s">
         <v>238</v>
       </c>
-      <c r="B107" t="s">
-        <v>561</v>
+      <c r="B107" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="C107" t="s">
         <v>240</v>
@@ -5851,13 +5854,13 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>89</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>90</v>
+        <v>238</v>
+      </c>
+      <c r="B108" t="s">
+        <v>561</v>
       </c>
       <c r="C108" t="s">
-        <v>91</v>
+        <v>240</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="10"/>
@@ -5869,7 +5872,7 @@
       </c>
       <c r="J108" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="K108" t="str">
         <f t="shared" si="12"/>
@@ -5878,13 +5881,13 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>193</v>
+        <v>89</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="C109" t="s">
-        <v>195</v>
+        <v>91</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="10"/>
@@ -5905,13 +5908,13 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>682</v>
-      </c>
-      <c r="B110" t="s">
-        <v>393</v>
+        <v>193</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="C110" t="s">
-        <v>681</v>
+        <v>195</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="10"/>
@@ -5927,18 +5930,18 @@
       </c>
       <c r="K110" t="str">
         <f t="shared" si="12"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>163</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>164</v>
+        <v>682</v>
+      </c>
+      <c r="B111" t="s">
+        <v>393</v>
       </c>
       <c r="C111" t="s">
-        <v>165</v>
+        <v>681</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="10"/>
@@ -5954,18 +5957,18 @@
       </c>
       <c r="K111" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>X</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>106</v>
+        <v>163</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
       <c r="C112" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="10"/>
@@ -5984,33 +5987,54 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>106</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C113" t="s">
+        <v>108</v>
+      </c>
+      <c r="H113" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="I113" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
       <c r="J113" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="K113" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J114" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J115" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J116" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C112">
-    <sortCondition ref="A2:A112"/>
+  <sortState ref="A2:C113">
+    <sortCondition ref="A2:A113"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12298,11 +12322,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -12578,154 +12606,154 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>449</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>705</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>202</v>
+        <v>9</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>203</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>155</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>394</v>
-      </c>
-      <c r="B39" t="s">
-        <v>393</v>
+        <v>75</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>25</v>
+        <v>394</v>
+      </c>
+      <c r="B40" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
-      <c r="B41" t="s">
-        <v>414</v>
+      <c r="B41" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>142</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>143</v>
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>172</v>
+        <v>57</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>173</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>257</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>149</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>148</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>199</v>
       </c>
-      <c r="B52" t="s">
-        <v>438</v>
+      <c r="B52" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>598</v>
+        <v>199</v>
       </c>
       <c r="B53" t="s">
-        <v>697</v>
+        <v>438</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -12733,470 +12761,478 @@
         <v>598</v>
       </c>
       <c r="B54" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>223</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>224</v>
+        <v>598</v>
+      </c>
+      <c r="B55" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>13</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>249</v>
+        <v>21</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>250</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>110</v>
+        <v>255</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>109</v>
       </c>
-      <c r="B61" t="s">
-        <v>489</v>
+      <c r="B61" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>211</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>212</v>
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>259</v>
+        <v>211</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>87</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>259</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>15</v>
       </c>
-      <c r="B67" t="s">
-        <v>463</v>
+      <c r="B67" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>118</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>119</v>
+        <v>15</v>
+      </c>
+      <c r="B68" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>128</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>196</v>
+        <v>127</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>197</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>508</v>
-      </c>
-      <c r="B72" t="s">
-        <v>507</v>
+        <v>196</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>6</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>7</v>
+        <v>508</v>
+      </c>
+      <c r="B73" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>166</v>
+        <v>6</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>167</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>208</v>
+        <v>151</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>209</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>701</v>
-      </c>
-      <c r="B78" t="s">
-        <v>635</v>
+        <v>208</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>214</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>215</v>
+        <v>701</v>
+      </c>
+      <c r="B79" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>548</v>
-      </c>
-      <c r="B81" t="s">
-        <v>547</v>
+        <v>252</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>229</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>230</v>
+        <v>548</v>
+      </c>
+      <c r="B82" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>268</v>
-      </c>
-      <c r="B83" t="s">
-        <v>695</v>
+        <v>229</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>184</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>185</v>
+        <v>268</v>
+      </c>
+      <c r="B84" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>568</v>
-      </c>
-      <c r="B85" t="s">
-        <v>567</v>
+        <v>184</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>175</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>176</v>
+        <v>568</v>
+      </c>
+      <c r="B86" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>602</v>
-      </c>
-      <c r="B87" t="s">
-        <v>601</v>
+        <v>175</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>187</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>188</v>
+        <v>602</v>
+      </c>
+      <c r="B88" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>206</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>217</v>
       </c>
-      <c r="B92" t="s">
-        <v>696</v>
+      <c r="B92" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>220</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
+      </c>
+      <c r="B93" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>98</v>
+        <v>221</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>620</v>
-      </c>
-      <c r="B95" t="s">
-        <v>619</v>
+        <v>97</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>51</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>52</v>
+        <v>620</v>
+      </c>
+      <c r="B96" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>631</v>
-      </c>
-      <c r="B97" t="s">
-        <v>630</v>
+        <v>51</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>517</v>
+        <v>631</v>
       </c>
       <c r="B98" t="s">
-        <v>702</v>
+        <v>630</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>657</v>
+        <v>517</v>
       </c>
       <c r="B99" t="s">
-        <v>656</v>
+        <v>702</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>27</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>28</v>
+        <v>657</v>
+      </c>
+      <c r="B100" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>264</v>
+        <v>27</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>669</v>
-      </c>
-      <c r="B102" t="s">
-        <v>704</v>
+        <v>264</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>18</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>19</v>
+        <v>669</v>
+      </c>
+      <c r="B103" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>232</v>
+        <v>40</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>233</v>
+        <v>41</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>238</v>
       </c>
-      <c r="B107" t="s">
-        <v>561</v>
+      <c r="B107" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>89</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>90</v>
+        <v>238</v>
+      </c>
+      <c r="B108" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>193</v>
+        <v>89</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>682</v>
-      </c>
-      <c r="B110" t="s">
-        <v>393</v>
+        <v>193</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>163</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>164</v>
+        <v>682</v>
+      </c>
+      <c r="B111" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>163</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>106</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>